<commit_message>
Worked on code formatting and organization.
</commit_message>
<xml_diff>
--- a/GUI Design for SafeSecrets.xlsx
+++ b/GUI Design for SafeSecrets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glenw\Dropbox\Personal\Hobbies\Software Dev Projects\JavaScript Projects\SafeSecrets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC006A9-1E72-48F6-AB11-AF4918534C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A44F04C-927B-4FAC-A53E-937FD220FA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7485" yWindow="240" windowWidth="12630" windowHeight="20295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,42 +106,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -198,19 +167,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -218,9 +184,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -243,15 +209,15 @@
 </file>
 
 <file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX11.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{978C9E23-D4B0-11CE-BF2D-00AA003F40D0}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
-<file path=xl/activeX/activeX11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX12.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
-</file>
-
-<file path=xl/activeX/activeX12.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{978C9E23-D4B0-11CE-BF2D-00AA003F40D0}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -259,11 +225,15 @@
 </file>
 
 <file path=xl/activeX/activeX14.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{978C9E23-D4B0-11CE-BF2D-00AA003F40D0}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX15.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{978C9E23-D4B0-11CE-BF2D-00AA003F40D0}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -271,19 +241,19 @@
 </file>
 
 <file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
-<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{978C9E23-D4B0-11CE-BF2D-00AA003F40D0}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
-<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX7.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D10-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
-</file>
-
-<file path=xl/activeX/activeX7.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -302,13 +272,13 @@
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>495300</xdr:colOff>
-          <xdr:row>40</xdr:row>
+          <xdr:row>35</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>42</xdr:row>
+          <xdr:row>37</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -360,13 +330,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
-          <xdr:row>7</xdr:row>
+          <xdr:row>2</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>123825</xdr:colOff>
-          <xdr:row>8</xdr:row>
+          <xdr:row>3</xdr:row>
           <xdr:rowOff>161925</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -418,13 +388,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
-          <xdr:row>10</xdr:row>
+          <xdr:row>5</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>29</xdr:row>
+          <xdr:row>24</xdr:row>
           <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -476,13 +446,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
-          <xdr:row>9</xdr:row>
+          <xdr:row>4</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>123825</xdr:colOff>
-          <xdr:row>10</xdr:row>
+          <xdr:row>5</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -534,13 +504,13 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>142875</xdr:colOff>
-          <xdr:row>8</xdr:row>
+          <xdr:row>3</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>10</xdr:row>
+          <xdr:row>5</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -592,13 +562,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
-          <xdr:row>40</xdr:row>
+          <xdr:row>35</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>295275</xdr:colOff>
-          <xdr:row>42</xdr:row>
+          <xdr:row>37</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -650,13 +620,13 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
-          <xdr:row>7</xdr:row>
+          <xdr:row>2</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>323850</xdr:colOff>
-          <xdr:row>8</xdr:row>
+          <xdr:row>3</xdr:row>
           <xdr:rowOff>161925</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -708,13 +678,13 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>342900</xdr:colOff>
-          <xdr:row>40</xdr:row>
+          <xdr:row>35</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>42</xdr:row>
+          <xdr:row>37</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -766,13 +736,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
-          <xdr:row>32</xdr:row>
+          <xdr:row>27</xdr:row>
           <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>40</xdr:row>
+          <xdr:row>35</xdr:row>
           <xdr:rowOff>57150</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -824,13 +794,13 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>571500</xdr:colOff>
-          <xdr:row>29</xdr:row>
+          <xdr:row>24</xdr:row>
           <xdr:rowOff>95250</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>30</xdr:row>
+          <xdr:row>25</xdr:row>
           <xdr:rowOff>142875</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -882,13 +852,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>29</xdr:row>
+          <xdr:row>24</xdr:row>
           <xdr:rowOff>123825</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>552450</xdr:colOff>
-          <xdr:row>30</xdr:row>
+          <xdr:row>25</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -940,13 +910,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>30</xdr:row>
+          <xdr:row>25</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>552450</xdr:colOff>
-          <xdr:row>32</xdr:row>
+          <xdr:row>27</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -998,13 +968,13 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>571500</xdr:colOff>
-          <xdr:row>30</xdr:row>
+          <xdr:row>25</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>32</xdr:row>
+          <xdr:row>27</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1054,16 +1024,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>266700</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>381000</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>7</xdr:col>
-          <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>152400</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>104775</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1074,6 +1044,64 @@
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D274081B-3D33-121B-E037-6AE00D654933}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>485774</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>123825</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>609599</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>104775</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1039" name="Label6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1039"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17980973-4679-1DF4-3DA1-4484AA847D6F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1378,7 +1406,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="B40" sqref="B40:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1389,7 +1417,9 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -1398,436 +1428,416 @@
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="7"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="10"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="8" t="s">
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="7"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="7"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="7"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="7"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="7"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="7"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="7"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="7"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="7"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="7"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="7"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="7"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="7"/>
-    </row>
-    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="11"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="13"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B2:G3"/>
-    <mergeCell ref="B6:G7"/>
-    <mergeCell ref="B4:G5"/>
+    <mergeCell ref="B1:G2"/>
+    <mergeCell ref="B40:G41"/>
+    <mergeCell ref="B42:G43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1835,44 +1845,69 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1038" r:id="rId3" name="Label5">
+        <control shapeId="1039" r:id="rId3" name="Label6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>266700</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>485775</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1038" r:id="rId3" name="Label5"/>
+        <control shapeId="1039" r:id="rId3" name="Label6"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId5" name="CommandButton1">
+        <control shapeId="1038" r:id="rId5" name="Label5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>381000</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>152400</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1038" r:id="rId5" name="Label5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId7" name="CommandButton1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>5</xdr:col>
                 <xdr:colOff>495300</xdr:colOff>
-                <xdr:row>40</xdr:row>
+                <xdr:row>35</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>42</xdr:row>
+                <xdr:row>37</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -1880,24 +1915,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId5" name="CommandButton1"/>
+        <control shapeId="1025" r:id="rId7" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId7" name="CommandButton2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+        <control shapeId="1026" r:id="rId9" name="CommandButton2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>7</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>76200</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>123825</xdr:colOff>
-                <xdr:row>8</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>161925</xdr:rowOff>
               </to>
             </anchor>
@@ -1905,24 +1940,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId7" name="CommandButton2"/>
+        <control shapeId="1026" r:id="rId9" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId9" name="TextBox1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+        <control shapeId="1027" r:id="rId11" name="TextBox1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>10</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>76200</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>29</xdr:row>
+                <xdr:row>24</xdr:row>
                 <xdr:rowOff>66675</xdr:rowOff>
               </to>
             </anchor>
@@ -1930,24 +1965,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId9" name="TextBox1"/>
+        <control shapeId="1027" r:id="rId11" name="TextBox1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId11" name="Label1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+        <control shapeId="1028" r:id="rId13" name="Label1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>9</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>123825</xdr:colOff>
-                <xdr:row>10</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>
             </anchor>
@@ -1955,24 +1990,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1028" r:id="rId11" name="Label1"/>
+        <control shapeId="1028" r:id="rId13" name="Label1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId13" name="TextBox2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+        <control shapeId="1029" r:id="rId15" name="TextBox2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>142875</xdr:colOff>
-                <xdr:row>8</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>180975</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>10</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
@@ -1980,24 +2015,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1029" r:id="rId13" name="TextBox2"/>
+        <control shapeId="1029" r:id="rId15" name="TextBox2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1030" r:id="rId15" name="CommandButton3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+        <control shapeId="1030" r:id="rId17" name="CommandButton3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>40</xdr:row>
+                <xdr:row>35</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>42</xdr:row>
+                <xdr:row>37</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -2005,24 +2040,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1030" r:id="rId15" name="CommandButton3"/>
+        <control shapeId="1030" r:id="rId17" name="CommandButton3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1031" r:id="rId17" name="CommandButton4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+        <control shapeId="1031" r:id="rId19" name="CommandButton4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>152400</xdr:colOff>
-                <xdr:row>7</xdr:row>
+                <xdr:row>2</xdr:row>
                 <xdr:rowOff>76200</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
                 <xdr:colOff>323850</xdr:colOff>
-                <xdr:row>8</xdr:row>
+                <xdr:row>3</xdr:row>
                 <xdr:rowOff>161925</xdr:rowOff>
               </to>
             </anchor>
@@ -2030,24 +2065,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1031" r:id="rId17" name="CommandButton4"/>
+        <control shapeId="1031" r:id="rId19" name="CommandButton4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1032" r:id="rId19" name="CommandButton5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+        <control shapeId="1032" r:id="rId21" name="CommandButton5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>342900</xdr:colOff>
-                <xdr:row>40</xdr:row>
+                <xdr:row>35</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>42</xdr:row>
+                <xdr:row>37</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -2055,24 +2090,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1032" r:id="rId19" name="CommandButton5"/>
+        <control shapeId="1032" r:id="rId21" name="CommandButton5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1033" r:id="rId21" name="Label2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
+        <control shapeId="1033" r:id="rId23" name="Label2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId24">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>32</xdr:row>
+                <xdr:row>27</xdr:row>
                 <xdr:rowOff>66675</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>40</xdr:row>
+                <xdr:row>35</xdr:row>
                 <xdr:rowOff>57150</xdr:rowOff>
               </to>
             </anchor>
@@ -2080,24 +2115,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1033" r:id="rId21" name="Label2"/>
+        <control shapeId="1033" r:id="rId23" name="Label2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1034" r:id="rId23" name="TextBox3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId24">
+        <control shapeId="1034" r:id="rId25" name="TextBox3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId26">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>571500</xdr:colOff>
-                <xdr:row>29</xdr:row>
+                <xdr:row>24</xdr:row>
                 <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>30</xdr:row>
+                <xdr:row>25</xdr:row>
                 <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
@@ -2105,24 +2140,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1034" r:id="rId23" name="TextBox3"/>
+        <control shapeId="1034" r:id="rId25" name="TextBox3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1035" r:id="rId25" name="Label3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId26">
+        <control shapeId="1035" r:id="rId27" name="Label3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId28">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>29</xdr:row>
+                <xdr:row>24</xdr:row>
                 <xdr:rowOff>123825</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>552450</xdr:colOff>
-                <xdr:row>30</xdr:row>
+                <xdr:row>25</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </to>
             </anchor>
@@ -2130,24 +2165,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1035" r:id="rId25" name="Label3"/>
+        <control shapeId="1035" r:id="rId27" name="Label3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1036" r:id="rId27" name="Label4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId28">
+        <control shapeId="1036" r:id="rId29" name="Label4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId30">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>30</xdr:row>
+                <xdr:row>25</xdr:row>
                 <xdr:rowOff>180975</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>552450</xdr:colOff>
-                <xdr:row>32</xdr:row>
+                <xdr:row>27</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
@@ -2155,24 +2190,24 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1036" r:id="rId27" name="Label4"/>
+        <control shapeId="1036" r:id="rId29" name="Label4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1037" r:id="rId29" name="TextBox4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId30">
+        <control shapeId="1037" r:id="rId31" name="TextBox4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>571500</xdr:colOff>
-                <xdr:row>30</xdr:row>
+                <xdr:row>25</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>32</xdr:row>
+                <xdr:row>27</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -2180,7 +2215,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1037" r:id="rId29" name="TextBox4"/>
+        <control shapeId="1037" r:id="rId31" name="TextBox4"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>